<commit_message>
Add the case with current nodes only and without voltage nodes
</commit_message>
<xml_diff>
--- a/ExamplePowerSystem_v3.xlsx
+++ b/ExamplePowerSystem_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backup H Drive\0 LYT temp\2020_12-xxxx Nature of Synchronization\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3B642A-82FD-4156-A7C9-504EA1C4150E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78941A4-2882-4046-8ABC-E640D46F2365}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1314,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>

</xml_diff>